<commit_message>
add correlation_analysis.csv and update dashboard.py
</commit_message>
<xml_diff>
--- a/Все csv.xlsx
+++ b/Все csv.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Груговая" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Гистограмма" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Таблица с данными" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="График рассеяния" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Статьи</t>
   </si>
@@ -63,6 +64,9 @@
   </si>
   <si>
     <t xml:space="preserve">Прибыль от услуг</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% влияния</t>
   </si>
 </sst>
 </file>
@@ -97,9 +101,12 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -961,4 +968,125 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2022</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2">
+        <f>C2/B2*100</f>
+        <v>109.09090909090908</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <f>C3/B3*100</f>
+        <v>88.888888888888886</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <f>C4/B4*100</f>
+        <v>116.66666666666667</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <f>C5/B5*100</f>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <f>C6/B6*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2">
+        <f>C7/B7*100</f>
+        <v>107.40740740740742</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>